<commit_message>
Draw horizontal ghosts on board
</commit_message>
<xml_diff>
--- a/boards/ThnderbirdEx1Board.xlsx
+++ b/boards/ThnderbirdEx1Board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ido\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tal Yamin\Desktop\Project\Thunderbirds\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEAD53F-5F5C-401C-8D0E-77C731837D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646517A7-83C3-4543-9F6C-F404D1DD1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2E380AA6-C73B-4A54-B2C0-24B88B62EC33}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2E380AA6-C73B-4A54-B2C0-24B88B62EC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="5">
   <si>
     <t>+</t>
   </si>
@@ -47,6 +46,9 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -126,7 +128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,7 +427,7 @@
   <dimension ref="A1:CB25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+      <selection activeCell="CA22" sqref="CA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,6 +1072,9 @@
       <c r="A20" t="s">
         <v>0</v>
       </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
       <c r="AI20" t="s">
         <v>0</v>
       </c>
@@ -1160,6 +1165,9 @@
       </c>
       <c r="BG22" t="s">
         <v>0</v>
+      </c>
+      <c r="CA22" t="s">
+        <v>4</v>
       </c>
       <c r="CB22" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fixes from Ido comments Still there is bug with first place of ghost is not empty
</commit_message>
<xml_diff>
--- a/boards/ThnderbirdEx1Board.xlsx
+++ b/boards/ThnderbirdEx1Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tal Yamin\Desktop\Project\Thunderbirds\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646517A7-83C3-4543-9F6C-F404D1DD1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2806727D-3F27-4266-8FE3-F883D73BB1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2E380AA6-C73B-4A54-B2C0-24B88B62EC33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="5">
   <si>
     <t>+</t>
   </si>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +84,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,11 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +435,7 @@
   <dimension ref="A1:CB25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CA22" sqref="CA22"/>
+      <selection activeCell="CB30" sqref="CB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,9 +968,6 @@
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="AH15" t="s">
-        <v>0</v>
-      </c>
       <c r="AI15" t="s">
         <v>0</v>
       </c>
@@ -1064,6 +1069,9 @@
       <c r="BE19" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="CA19" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="CB19" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1080,7 @@
       <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="AI20" t="s">
@@ -1165,9 +1173,6 @@
       </c>
       <c r="BG22" t="s">
         <v>0</v>
-      </c>
-      <c r="CA22" t="s">
-        <v>4</v>
       </c>
       <c r="CB22" t="s">
         <v>0</v>

</xml_diff>